<commit_message>
Upload Sequence sheets with 'Answer' in Integer format
</commit_message>
<xml_diff>
--- a/runs/seq_1_2_ic.xlsx
+++ b/runs/seq_1_2_ic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanos\Documents\Work\Columbia Research Assistant Job\PsychoPy Experiments\Cocaine_Study_Stroop_Test\runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12234D61-7C13-4023-825F-203D4ED56502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BEFDFC-EE8C-4737-A24C-4F284DC91235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{404563F4-4C40-704E-ADCD-BBD7885789F8}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{404563F4-4C40-704E-ADCD-BBD7885789F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,19 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="14">
-  <si>
-    <t>'5'</t>
-  </si>
-  <si>
-    <t>'4'</t>
-  </si>
-  <si>
-    <t>'3'</t>
-  </si>
-  <si>
-    <t>'2'</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="10">
   <si>
     <t>type</t>
   </si>
@@ -457,981 +445,981 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CBA18CA-4CB6-DD4B-95C7-D894594388BB}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.84765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.1484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D3" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D12" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D15" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D16" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D17" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D20" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D21" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>2</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D23" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C24">
         <v>3</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D24" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D25" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D26" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D27" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C28">
         <v>2</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>2</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D31" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C32">
         <v>2</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D33" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D34" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D35" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D36" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D37" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C39">
         <v>3</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D39" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C40">
         <v>3</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D40" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D41" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C42">
         <v>4</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D42" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C43">
         <v>2</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D43" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C44">
         <v>2</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D44" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D45" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C46">
         <v>3</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D46" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D47" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C48">
         <v>4</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D48" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D49" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D50" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C51">
         <v>4</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D51" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C52">
         <v>3</v>
       </c>
-      <c r="D52" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D52" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C53">
         <v>4</v>
       </c>
-      <c r="D53" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D53" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
-      <c r="D54" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D54" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C55">
         <v>4</v>
       </c>
-      <c r="D55" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D55" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C56">
         <v>2</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D56" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C57">
         <v>3</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D57" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C58">
         <v>4</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D58" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C59">
         <v>3</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D59" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C60">
         <v>2</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D60" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B61" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <v>3</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D61" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C62">
         <v>4</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D62" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C63">
         <v>2</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D63" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C64">
         <v>3</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D64" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B65" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D65" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B66" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C66">
         <v>4</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D66" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C67">
         <v>2</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D67" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C68">
         <v>4</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.6">
+      <c r="D68" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C69">
         <v>4</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>0</v>
+      <c r="D69" s="3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>